<commit_message>
fix bootstrap location in macs/win8.1
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BAC182-48DE-430F-8AF1-75CFEF51FBD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63F73E5-D214-4E16-86EB-15F74ADBFC46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26850" yWindow="1275" windowWidth="14280" windowHeight="9045" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40200" yWindow="960" windowWidth="14280" windowHeight="9045" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -521,9 +521,6 @@
   </si>
   <si>
     <t>mac-4-03.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h2&gt;&lt;a name="eset"&gt;&lt;/a&gt;ESET Endpoint Antivitudの手動更新とフルスキャン&lt;/h2&gt; </t>
   </si>
   <si>
     <t>mac-4-04.svg</t>
@@ -1180,6 +1177,10 @@
   </si>
   <si>
     <t>mac-1-02a.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2&gt;&lt;a name="eset"&gt;&lt;/a&gt;ESET Endpoint Antivirusの手動更新とフルスキャン&lt;/h2&gt; </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1604,7 +1605,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -1612,7 +1613,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1678,7 +1679,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -1928,7 +1929,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -1964,13 +1965,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2081,7 +2082,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2233,7 +2234,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="156" x14ac:dyDescent="0.2">
@@ -2260,7 +2261,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2293,13 +2294,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -2313,7 +2314,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2321,13 +2322,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2443,7 +2444,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -2583,7 +2584,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -2597,7 +2598,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -2667,7 +2668,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -2700,7 +2701,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -2719,8 +2720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2760,7 +2761,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2787,7 +2788,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2801,7 +2802,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -2815,7 +2816,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -2826,7 +2827,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2834,13 +2835,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2848,13 +2849,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2862,13 +2863,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2876,18 +2877,18 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2895,13 +2896,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2909,13 +2910,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2923,13 +2924,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2937,13 +2938,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2951,13 +2952,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2965,13 +2966,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2979,13 +2980,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2993,13 +2994,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3007,13 +3008,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3021,13 +3022,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3035,13 +3036,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3049,13 +3050,13 @@
         <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3069,8 +3070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3086,7 +3087,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3094,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3110,7 +3111,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -3118,7 +3119,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3129,7 +3130,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3151,13 +3152,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>153</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3165,18 +3166,18 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>155</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3198,13 +3199,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>158</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3212,21 +3213,21 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>160</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D15" t="s">
         <v>230</v>
-      </c>
-      <c r="D15" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3234,13 +3235,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>232</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3248,13 +3249,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" t="s">
         <v>162</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>163</v>
-      </c>
-      <c r="D17" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3262,13 +3263,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" t="s">
         <v>165</v>
-      </c>
-      <c r="C18" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3276,13 +3277,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
         <v>167</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3290,13 +3291,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
         <v>169</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3304,18 +3305,18 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
         <v>171</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3337,13 +3338,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
         <v>174</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3351,13 +3352,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
         <v>176</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3365,18 +3366,18 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
         <v>178</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3398,13 +3399,13 @@
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
         <v>181</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3412,13 +3413,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
         <v>183</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3426,13 +3427,13 @@
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
         <v>185</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3440,13 +3441,13 @@
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
         <v>187</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -3454,13 +3455,13 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
         <v>189</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3468,13 +3469,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
         <v>191</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3482,13 +3483,13 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
         <v>193</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3496,13 +3497,13 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
         <v>195</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3510,13 +3511,13 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
         <v>197</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3524,18 +3525,18 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>199</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3543,7 +3544,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -3557,13 +3558,13 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3571,13 +3572,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3585,13 +3586,13 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3599,13 +3600,13 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3619,8 +3620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3636,7 +3637,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3652,7 +3653,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3660,7 +3661,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3671,12 +3672,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="117" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3684,7 +3685,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -3695,7 +3696,7 @@
     </row>
     <row r="9" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix mac-4-16a svg->png(display size problem)
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63F73E5-D214-4E16-86EB-15F74ADBFC46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9889F6A-AB1F-484F-BC63-F6D9CD4AA948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40200" yWindow="960" windowWidth="14280" windowHeight="9045" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="1890" windowWidth="14280" windowHeight="9045" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -1108,10 +1108,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>mac-4-16a.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>mac-2-02a.svg</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1181,6 +1177,10 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="eset"&gt;&lt;/a&gt;ESET Endpoint Antivirusの手動更新とフルスキャン&lt;/h2&gt; </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mac-4-16a.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1971,7 +1971,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2300,7 +2300,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -2314,7 +2314,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2322,13 +2322,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2444,7 +2444,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -2584,7 +2584,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -2598,7 +2598,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -2720,8 +2720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3042,7 +3042,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
copy report from win10_en -> macs/win8.1
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9889F6A-AB1F-484F-BC63-F6D9CD4AA948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC9AF83-92F9-41B5-B35E-C20661326EDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="1890" windowWidth="14280" windowHeight="9045" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="1890" windowWidth="14280" windowHeight="9045" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -2720,8 +2720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3039,7 +3039,7 @@
         <v>250</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D27" t="s">
         <v>261</v>
@@ -3070,8 +3070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
win10/macs add USBinstall protocol
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF0160E-CBCB-408D-9BF5-C5BE9B05E6A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7B9E8B-4EEC-43C5-B583-04DBE338EBCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35760" yWindow="1065" windowWidth="18225" windowHeight="11625" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2500" yWindow="1400" windowWidth="13500" windowHeight="8270" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="ch5" sheetId="6" r:id="rId7"/>
     <sheet name="ch6" sheetId="7" r:id="rId8"/>
     <sheet name="ch7" sheetId="8" r:id="rId9"/>
+    <sheet name="ch8" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="301">
   <si>
     <t>header1</t>
   </si>
@@ -1064,10 +1065,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win10-4-24.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>このページの説明をひととおり下まで読んでから、左側メニューの「各種ソフトウェアのダウンロード」をクリックします。</t>
     <rPh sb="6" eb="8">
       <t>セツメイ</t>
@@ -1083,63 +1080,6 @@
     </rPh>
     <rPh sb="31" eb="33">
       <t>カクシュ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「学生の個人所有PCへのインストールはここから」をクリック、さらに表示されるページにある「個人所有PCのOffice製品は、Office365 Pro Plusをご利用ください」をクリックします。</t>
-    <rPh sb="1" eb="3">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ショユウ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>ショユウ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>セイヒン</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>リヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-4-22.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「職場または学校アカウントでサインインする」には広大メールアドレス（ IMCアカウント名@hiroshima-u.ac.jp ）を入力してください。パスワードには広大パスワードを入力します。</t>
-    <rPh sb="1" eb="3">
-      <t>ショクバ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ガッコウ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="81" eb="83">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="89" eb="91">
-      <t>ニュウリョク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1254,10 +1194,6 @@
   </si>
   <si>
     <t xml:space="preserve">ここで Officeのアップデートの方法を説明します。 Officeのソフトのどれでもいいのですが、上のメニューから「ヘルプ」をクリックしてください。 「更新プログラムのチェック」をクリックしてください。  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>mac-2-31.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1286,42 +1222,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>このページの「ESET for Mac」をクリックすると、インストール手順を書いたマニュアルが表示されます。
-ひととおり下まで読んでから、先ほどのページに戻ってください。
-&lt;p class="spl"&gt;※ できればこのマニュアルを別ウィンドウで表示したままにしておくと、あとの作業がやりやすいでしょう。&lt;/p&gt;</t>
-    <rPh sb="35" eb="37">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="60" eb="61">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>モド</t>
-    </rPh>
-    <rPh sb="115" eb="116">
-      <t>ベツ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="138" eb="140">
-      <t>サギョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>左側メニューの「各種ソフトウェアのダウンロード」をクリックします。</t>
     <rPh sb="0" eb="2">
       <t>ヒダリガワ</t>
@@ -1404,10 +1304,6 @@
     <t xml:space="preserve">さきほどのOfficeの時と同様、使用許諾契約の段階に入ります。「続ける」をクリックしてください。 
 &lt;p class="spl"&gt;※本来は表示されている利用許諾契約をひととおり読んでから同意するものです&lt;/p&gt;
   </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-41.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1430,20 +1326,6 @@
   <si>
     <t>win10-2-42.png</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ダウンロードしたファイルを実行します。</t>
-    <rPh sb="13" eb="15">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-43.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-11.svg</t>
   </si>
   <si>
     <t xml:space="preserve">次にGoogle Chromeをインストールします。Web上の配布サイトから直接ダウンロードしましょう。
@@ -1572,20 +1454,293 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">右図のような表示が出るので、Chromeのアイコンを下に見えている「A」のついたフォルダにドラッグしてコピーしてください。Chromeのインストールはこれで終了です。
-&lt;p class="spl"&gt; ※ macOSにはSafariというWebブラウザが標準的なものとして付属してきますが、うまく表示できないWebページもときどきあります。そういうときに、「もう一つのブラウザ」としてこのChromeを使ってみてください。&lt;/p&gt;  </t>
+    <t>description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>必携PC使用時の問い合わせ窓口と、PC活用講習会（F3S講習会）を案内します。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒッケイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>マドグチ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>カツヨウ</t>
+    </rPh>
+    <rPh sb="21" eb="24">
+      <t>コウシュウカイ</t>
+    </rPh>
+    <rPh sb="28" eb="31">
+      <t>コウシュウカイ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>アンナイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インターネットからのソフトウェアダウンロードがうまくいかない場合は、メディアセンターで借りられる配布用USBメモリを使います。</t>
+    <rPh sb="30" eb="32">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ハイフ</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（付録A）USBメモリからのソフトウェアインストール</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2020 Mac App.A</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2&gt;&lt;a name="copy"&gt;&lt;/a&gt;USBメモリからファイルをコピーする&lt;/h2&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">配布されたUSBメモリをUSBポートに挿します。 
+  </t>
+  </si>
+  <si>
+    <t>mac-2-1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">デスクトップに、USBメモリの内容を表す「FIRST LEC」が現れますので、ダブルクリックして開きましょう。
+ 中にある「setup2020-mac」フォルダをデスクトップにドラッグしてコピーします。   </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mac-2-02a.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">コピーが終了したら「FIRST LEC」をゴミ箱までドラッグ＆ドロップしてください。ドラッグを始めると、ゴミ箱がイジェクトアイコンに 変わります。
+デスクトップから「FIRST LEC」のアイコンが消えたらUSBメモリを抜き、次の人に回してください。
+&lt;div class="spl"&gt;※ イジェクトの動作は、「FIRST LEC」のアイコンを右クリックして、「&amp;quot;FIRST LEC&amp;quot;を取り出す」としてもOKです。
+ちなみに右クリックは、controlキーを押しながらクリックします。「システム環境設定」の「トラックパッド」の項目を開くと、他のやり方を設定できます。
+&lt;/div&gt;
+   </t>
+  </si>
+  <si>
+    <t>mac-2-03.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">デスクトップの「mac」フォルダを開きましょう。4つのファイルが入っています。そのうち3つを順に入れていきます。 &lt;ul&gt;&lt;li&gt;officemac.pkg: Microsoft Office &lt;/li&gt;
+&lt;li&gt;eset_osx_ja.dmg: Microsoftのウィルス対策ソフト &lt;/li&gt;
+&lt;li&gt;googlechrome.dmg: Google Chrome (Webブラウザ) &lt;/li&gt;
+&lt;/ul&gt;
+ </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mac-2-04a.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2&gt;&lt;a name="office"&gt;&lt;/a&gt;Officeを入れる&lt;/h2&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まずMicrosoft Officeをインストールしましょう。WordとExcelとPowerPointを中心とした業務用アプリケーションセットです。大学でもよく使います。
+ Ofiice.pkg をダブルクリックします。インストーラのウィンドウが出ますので「続ける」をクリックしてください。 Officeのインスールは特に悩ましい分かれ道はありませんので、基本的に前に進む方向の選択肢を選んでいけばOKです。   </t>
+  </si>
+  <si>
+    <t>mac-2-4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">使用許諾契約をはじめます。「続ける」をクリックしてください。 
+  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">実際にインストーラからファイルを書き込むステップに入ります。「インストール」をクリックしてください。 
+  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macのシステム領域にファイルを書き込みますので、管理者権限を持っている利用者であることを確認するため、認証を求められます。6ページで作った利用者名とパスワードを入力してください。広大パスワードではないので、間違えないように。 
+  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">しばらくまつと、ポロリンと音がなり、このような画面になります。「閉じる」をクリックしてインストーラを終了させましょう。
+&lt;p class="spl"&gt;※ インストールは終了ですが、この段階ではまだ使えません。使い始めるには「ライセンス認証」が必要です。それには、インターネットに接続されていることが必要ですので、のちほど行います。 &lt;/p&gt;
+  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">次に、ウィルス対策ソフトのESET Endpoint Antivirus (以下 ESET EA) をインストールします。
+ まず、USBメモリからコピーしたフォルダにある eset_osx_ja.pkg をダブルクリック。インストーラが立ち上がります。  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">さきほどのOfficeの時と同様、使用許諾契約の段階に入ります。「続ける」をクリックしてください。 
+  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">「同意する」をクリックしてください。しないと先に進めません... 
+  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macにログインするときに使うパスワードを入力し、「ソフトウェアをインストール」としてください。 このあと特に警告が出なければ、[31]のChromeを入れる手順に進んでかまいません。
+  </t>
+    <rPh sb="53" eb="54">
+      <t>トク</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ケイコク</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="82" eb="83">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">次にChromeをインストールしましょう。googlechrome.dmgをダブルクリックすると、Chromeが入っているフォルダが開きます。これを下に見えている「A」のついたフォルダにドラッグしてコピーしてください。Chromeのインストールはこれで終了です。
+&lt;p class="spl"&gt; ※ macOSにはSafariというWebブラウザが標準的なものとして付属してきますが、うまく表示できないWebページもときどきあります。そういうときに、「もう一つのブラウザ」としてこのChromeを使ってみてください。&lt;/p&gt;
+&lt;p class="spl"&gt;※ (今はまあどうでもいいこと）「A」のフォルダの左下に小さな矢印がついていますね。Macでは、フォルダやファイルの実体とは別の場所に、その実体と同じ動作をするようなものを作ることができます。その影武者のような項目を「エイリアス」と呼びます。左下の矢印は、この項目がエイリアスであることを示しています。右クリックして「オリジナルを表示」とすると、この項目が、あなたのMacの「アプリケーション」フォルダのエイリアスであることがわかります。 &lt;/p&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mac-2-23.png</t>
+  </si>
+  <si>
+    <t>ここでは、第３章、第４章で説明しているソフトウェアのダウンロードがうまくいかない場合に、メディアセンターで配布用USBを借りてソフトウェアをインストールする方法を説明します。
+&lt;ul&gt;&lt;li&gt;&lt;a href="#copy"&gt;USBメモリからファイルをコピーする&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#office"&gt;Officeを入れる&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#eset"&gt;ESET EAを入れる&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#chrome"&gt;Chromeを入れる&lt;/a&gt;
+&lt;/li&gt;
+ &lt;/ul&gt;</t>
+    <rPh sb="5" eb="6">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>ハイフ</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="60" eb="61">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-4-24.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-4-22.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-4-21.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>右のような画面になるので、「個人所有PCのOffice製品は、Office365 Pro Plusをご利用ください」をクリックします。</t>
     <rPh sb="0" eb="1">
       <t>ミギ</t>
     </rPh>
-    <rPh sb="1" eb="2">
+    <rPh sb="5" eb="7">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ショユウ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>セイヒン</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>リヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-4-25.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mac-4-11.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ダウンロードしたファイルを実行すると右図のような表示が出るので、Chromeのアイコンを下に見えている「A」のついたフォルダにドラッグしてコピーしてください。Chromeのインストールはこれで終了です。
+&lt;p class="spl"&gt; ※ macOSにはSafariというWebブラウザが標準的なものとして付属してきますが、うまく表示できないWebページもときどきあります。そういうときに、「もう一つのブラウザ」としてこのChromeを使ってみてください。&lt;/p&gt;  </t>
+    <rPh sb="18" eb="19">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
       <t>ズ</t>
     </rPh>
-    <rPh sb="6" eb="8">
+    <rPh sb="24" eb="26">
       <t>ヒョウジ</t>
     </rPh>
-    <rPh sb="9" eb="10">
+    <rPh sb="27" eb="28">
       <t>デ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-2-41.ｓｖｇ</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2047,6 +2202,540 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF271FC4-129F-4F71-9511-33294FAB9AAD}">
+  <dimension ref="A1:D44"/>
+  <sheetViews>
+    <sheetView topLeftCell="C36" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="130" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D18"/>
@@ -2587,9 +3276,429 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" zoomScale="113" workbookViewId="0">
+    <sheetView topLeftCell="B29" zoomScale="113" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D13" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACFDDE6-1E06-4807-90D9-56730BF2F634}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="138" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -2606,7 +3715,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2614,7 +3723,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2630,401 +3739,6 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="117" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D12" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C32" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>124</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACFDDE6-1E06-4807-90D9-56730BF2F634}">
-  <dimension ref="A1:D36"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="138" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3033,7 +3747,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3049,55 +3763,73 @@
     </row>
     <row r="8" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
       <c r="B9" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>256</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3105,83 +3837,83 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>255</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>260</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3189,55 +3921,55 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>88</v>
+        <v>251</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3245,140 +3977,118 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>224</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>98</v>
+        <v>200</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>200</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+      <c r="D32" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="D33" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
       <c r="B34" s="1" t="s">
-        <v>263</v>
+        <v>299</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D35" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -3440,7 +4150,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3534,7 +4244,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -3548,7 +4258,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -3568,8 +4278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3609,7 +4319,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -4116,10 +4826,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4132,73 +4842,82 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="117" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="104" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update win10e to self studying ver.
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB01C0AF-15F1-466C-8C15-CC7FBC7E13E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50BB313-7CB8-415B-9AE3-60A051F0D916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26880" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="2280" windowWidth="17000" windowHeight="7770" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -610,29 +610,7 @@
     <t>win10-6-16.svg</t>
   </si>
   <si>
-    <t xml:space="preserve">2回目からはログインしたら、この画面が出ます。
-真ん中の「コース一覧」に、あなたがアクセスできるコースが表示されています。
-ここに並んでいるコースは、あなたが受講する授業に関連したものと、そうでないものがあります。今並んでいるものを簡単に説明すると：
-&lt;dl&gt;&lt;dt&gt;大学教育入門&lt;/dt&gt;
-&lt;dd&gt;「大学教育入門」は、大学で学ぶにあたり必要な事柄や、広島大学特有の事情について学習する授業です。全学部生必修です。このコースでは、授業の各週で使う資料をダウンロードしたり、確認テストを受験したりします。&lt;/dd&gt;
-&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
-&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届け」を提出する必要があります。このコースでは、点検届けが提出できます。この講習会のあとで各自開いて実施してください。&lt;/dd&gt;
-&lt;dt&gt;Information Security and Compliance (情報セキュリティ・コンプライアンス)&lt;/dt&gt;
-&lt;dd&gt;「情報セキュリティ・コンプライアンス講習」は、広島大学でパソコンやネットワークを安全に使うための講座です。学生だけでなく、教職員を含めた全構成員必修の内容です。講習は、教室での講義とオンライン学習（このコース）からなっています。6月末までにこのコースの中にある確認テストに合格し、「&lt;em&gt;アカウント利用確認&lt;/em&gt;
-」の手続きをおこなわないと、アカウントがロックされ、メール等が使えなくなります。&lt;/dd&gt;
- &lt;/dl&gt;
-  </t>
-  </si>
-  <si>
     <t>win10-6-17.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bb9で配布されている教材を開けることを確認するため、「大学教育入門」のコースをみてみましょう。
-転入生の方は、「大学教育入門」がありませんので、「Information Security and Compliance」のコースを開いて、スライドなどがみられることを確認してください。
-「大学教育入門」では、授業に参加する前に各自必携PCに教材をダウンロードしておくことが求められています。先ほど開いたメールにその旨の指示が来ていたと思います。
-ここでは、第1週に実施される講義の資料をダウンロードする手順を紹介しておきます。
-まず、コース一覧から「2019大学教育入門...」をクリックしてコースを開きましょう。
-  </t>
   </si>
   <si>
     <t>win10-6-18.svg</t>
@@ -759,44 +737,6 @@
 2020年4月&lt;br&gt;
  広島大学 情報メディア教育研究センター&lt;br&gt;
  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>必携PCを使っていて、わからないことや困ったことがあったら、情報メディア教育研究センターに相談してください。
-&lt;dl&gt;&lt;dt&gt;対面窓口&lt;/dt&gt;
-&lt;dt&gt; &lt;/dt&gt;
-&lt;dd&gt;メディアセンター本館、東分室（東図書館内）、サービスデスク（西図書館内、中央図書館内）、霞分室（基礎講義棟1F）&lt;/dd&gt;
-&lt;dd&gt;&lt;a href="https://www.media.hiroshima-u.ac.jp/helpdesk"&gt;アクセスマップ&lt;/a&gt;&lt;/dd&gt;&lt;dt&gt;Web質問窓口: &lt;/dt&gt;
-&lt;dt&gt; &lt;/dt&gt;
-&lt;dd&gt;&lt;a href="https://www.media.hiroshima-u.ac.jp/helpdesk"&gt;https://www.media.hiroshima-u.ac.jp/helpdesk&lt;/a&gt;
-&lt;/dd&gt;</t>
-    <rPh sb="99" eb="100">
-      <t>ヒガシ</t>
-    </rPh>
-    <rPh sb="100" eb="102">
-      <t>ブンシツ</t>
-    </rPh>
-    <rPh sb="103" eb="104">
-      <t>ヒガシ</t>
-    </rPh>
-    <rPh sb="104" eb="107">
-      <t>トショカン</t>
-    </rPh>
-    <rPh sb="107" eb="108">
-      <t>ナイ</t>
-    </rPh>
-    <rPh sb="122" eb="123">
-      <t>ナイ</t>
-    </rPh>
-    <rPh sb="124" eb="126">
-      <t>チュウオウ</t>
-    </rPh>
-    <rPh sb="126" eb="129">
-      <t>トショカン</t>
-    </rPh>
-    <rPh sb="129" eb="130">
-      <t>ナイ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1815,6 +1755,129 @@
     <rPh sb="19" eb="21">
       <t>ハイフ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>必携PCの設定・点検についてわからないことや困ったことがあったら、下記窓口に相談してください。
+&lt;dl&gt;&lt;dt&gt;対面窓口&lt;/dt&gt;
+&lt;dt&gt; &lt;/dt&gt;
+&lt;dd&gt;初期講習会会場（日時場所は下記Webページ内）&lt;/dd&gt;
+&lt;dd&gt;&lt;a href="https://info.pre-entrance.hiroshima-u.ac.jp/"&gt;https://info.pre-entrance.hiroshima-u.ac.jp/&lt;/a&gt;&lt;/dd&gt;
+&lt;dd&gt;（4/4～5 13:00～17:00）メディアセンター本館特設会場&lt;/dd&gt;
+&lt;dd&gt;（平日 8:45～16:45）メディアセンター本館、東分室（東図書館内）、サービスデスク（西図書館内、中央図書館内）、霞分室（基礎講義棟1F）&lt;/dd&gt;
+&lt;dd&gt;&lt;a href="https://www.media.hiroshima-u.ac.jp/helpdesk"&gt;アクセスマップ&lt;/a&gt;
+&lt;dd&gt;（4/4～5 10:00～19:00、平日 10:00～17:00）広島大学生協新入生サポートセンター&lt;/dd&gt;
+&lt;/dd&gt;&lt;dt&gt;Web質問窓口: &lt;/dt&gt;
+&lt;dt&gt; &lt;/dt&gt;
+&lt;dd&gt;&lt;a href="https://www.media.hiroshima-u.ac.jp/helpdesk"&gt;https://www.media.hiroshima-u.ac.jp/helpdesk&lt;/a&gt;
+&lt;/dd&gt;&lt;dt&gt;メール質問窓口: &lt;/dt&gt;
+&lt;dt&gt; &lt;/dt&gt;
+&lt;dd&gt;&lt;a href="mailto:st-pc@ml.hiroshima-u.ac.jp"&gt;st-pc@ml.hiroshima-u.ac.jp&lt;/a&gt;&lt;/dd&gt;</t>
+    <rPh sb="5" eb="7">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>カキ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>マドグチ</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>ショキ</t>
+    </rPh>
+    <rPh sb="83" eb="86">
+      <t>コウシュウカイ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>カイジョウ</t>
+    </rPh>
+    <rPh sb="89" eb="91">
+      <t>ニチジ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>バショ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>カキ</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="256" eb="258">
+      <t>トクセツ</t>
+    </rPh>
+    <rPh sb="258" eb="260">
+      <t>カイジョウ</t>
+    </rPh>
+    <rPh sb="271" eb="273">
+      <t>ヘイジツ</t>
+    </rPh>
+    <rPh sb="296" eb="297">
+      <t>ヒガシ</t>
+    </rPh>
+    <rPh sb="297" eb="299">
+      <t>ブンシツ</t>
+    </rPh>
+    <rPh sb="300" eb="301">
+      <t>ヒガシ</t>
+    </rPh>
+    <rPh sb="301" eb="304">
+      <t>トショカン</t>
+    </rPh>
+    <rPh sb="304" eb="305">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="319" eb="320">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="321" eb="323">
+      <t>チュウオウ</t>
+    </rPh>
+    <rPh sb="323" eb="326">
+      <t>トショカン</t>
+    </rPh>
+    <rPh sb="326" eb="327">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="456" eb="458">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="458" eb="460">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="460" eb="462">
+      <t>セイキョウ</t>
+    </rPh>
+    <rPh sb="462" eb="465">
+      <t>シンニュウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2回目からはログインしたら、この画面が出ます。
+真ん中の「コース一覧」に、あなたがアクセスできるコースが表示されています。
+ここに並んでいるコースは、あなたが受講する授業に関連したものと、そうでないものがあります。今並んでいるものを簡単に説明すると：
+&lt;dl&gt;&lt;dt&gt;大学教育入門&lt;/dt&gt;
+&lt;dd&gt;「大学教育入門」は、大学で学ぶにあたり必要な事柄や、広島大学特有の事情について学習する授業です。全学部生必修です。このコースでは、授業の各週で使う資料をダウンロードしたり、確認テストを受験したりします。&lt;/dd&gt;
+&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
+&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届け」を提出する必要があります。このコースでは、点検届けが提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
+&lt;dt&gt;Information Security and Compliance (情報セキュリティ・コンプライアンス)&lt;/dt&gt;
+&lt;dd&gt;「情報セキュリティ・コンプライアンス講習」は、広島大学でパソコンやネットワークを安全に使うための講座です。学生だけでなく、教職員を含めた全構成員必修の内容です。講習は、教室での講義とオンライン学習（このコース）からなっています。6月末までにこのコースの中にある確認テストに合格し、「&lt;em&gt;アカウント利用確認&lt;/em&gt;
+」の手続きをおこなわないと、アカウントがロックされ、メール等が使えなくなります。&lt;/dd&gt;
+ &lt;/dl&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Bb9で配布されている教材を開けることを確認するため、「大学教育入門」のコースをみてみましょう。
+転入生の方は、「大学教育入門」がありませんので、「Information Security and Compliance」のコースを開いて、スライドなどがみられることを確認してください。
+「大学教育入門」では、授業に参加する前に各自必携PCに教材をダウンロードしておくことが求められています。先ほど開いたメールにその旨の指示が来ていたと思います。
+ここでは、第1週に実施される講義の資料をダウンロードする手順を紹介しておきます。
+まず、コース一覧から「2020大学教育入門...」をクリックしてコースを開きましょう。
+  </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2223,7 +2286,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2239,7 +2302,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2247,7 +2310,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -2298,7 +2361,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2306,7 +2369,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2322,7 +2385,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2330,7 +2393,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2341,7 +2404,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2349,13 +2412,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2363,13 +2426,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -2377,13 +2440,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2391,18 +2454,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2410,13 +2473,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2424,7 +2487,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2452,7 +2515,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -2466,7 +2529,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2494,7 +2557,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2513,7 +2576,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -2569,7 +2632,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -2583,7 +2646,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -2653,7 +2716,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -2667,7 +2730,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -2737,7 +2800,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -2770,13 +2833,13 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2784,7 +2847,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -2832,7 +2895,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2856,7 +2919,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3106,7 +3169,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3142,13 +3205,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3259,12 +3322,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3272,7 +3335,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3286,7 +3349,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -3379,7 +3442,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3387,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3403,7 +3466,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3411,7 +3474,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3422,12 +3485,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3435,13 +3498,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3449,13 +3512,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3463,37 +3526,37 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D12" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D13" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3501,18 +3564,18 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3520,7 +3583,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -3548,7 +3611,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -3562,7 +3625,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -3590,7 +3653,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -3601,7 +3664,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3609,7 +3672,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -3623,7 +3686,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -3637,7 +3700,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -3651,7 +3714,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -3665,7 +3728,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -3679,7 +3742,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -3693,7 +3756,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -3707,7 +3770,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -3721,7 +3784,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -3735,7 +3798,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -3749,13 +3812,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -3763,7 +3826,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -3782,7 +3845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACFDDE6-1E06-4807-90D9-56730BF2F634}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="138" workbookViewId="0">
+    <sheetView topLeftCell="B15" zoomScale="138" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3799,7 +3862,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3807,7 +3870,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3823,7 +3886,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3831,7 +3894,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3847,18 +3910,18 @@
     </row>
     <row r="8" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D9" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3866,13 +3929,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3882,10 +3945,10 @@
     </row>
     <row r="12" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3893,34 +3956,34 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D15" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3928,7 +3991,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -3956,7 +4019,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -3984,7 +4047,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -3998,7 +4061,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -4068,7 +4131,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -4082,7 +4145,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -4152,7 +4215,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -4227,7 +4290,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4235,7 +4298,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4254,7 +4317,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -4268,7 +4331,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -4282,7 +4345,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -4293,7 +4356,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4301,7 +4364,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -4315,7 +4378,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -4329,7 +4392,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -4343,7 +4406,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -4363,8 +4426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4404,7 +4467,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -4412,7 +4475,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4517,10 +4580,10 @@
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4528,13 +4591,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4748,13 +4811,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
         <v>162</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4762,13 +4825,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>164</v>
+        <v>302</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4776,13 +4839,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4790,13 +4853,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4804,13 +4867,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4818,18 +4881,18 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4837,7 +4900,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -4851,13 +4914,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4865,13 +4928,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C42" t="s">
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4879,13 +4942,13 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -4893,13 +4956,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4913,8 +4976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4927,10 +4990,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4938,7 +5001,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4954,7 +5017,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4962,7 +5025,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4973,12 +5036,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>196</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4986,7 +5049,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -4997,7 +5060,7 @@
     </row>
     <row r="10" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix checklist No., fix win10e Ch. 0
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50BB313-7CB8-415B-9AE3-60A051F0D916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508AC9D9-0AB9-43FC-95D4-48D76A328E96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="2280" windowWidth="17000" windowHeight="7770" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29295" yWindow="2070" windowWidth="17925" windowHeight="12450" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -204,11 +204,6 @@
     <t>mac-1-05.svg</t>
   </si>
   <si>
-    <t xml:space="preserve">アクティビティモニタのウィンドウで、まず「エネルギー」タブをクリックしてください。
- この画面の下の方に、現在のバッテリー情報がかかれています。あと4時間40分使えるとあります。充電状況が100%のときにこの「残り時間」を調べれば、それがあなたのMacのバッテリー駆動時間ということになります。&lt;span class="check"&gt;check-3&lt;/span&gt;
- この数字は推測値であり、プログラムの動作状況によって大きく上下することに注意してください。   </t>
-  </si>
-  <si>
     <t>mac-1-06.svg</t>
   </si>
   <si>
@@ -246,11 +241,6 @@
     <t>mac-3-3.png</t>
   </si>
   <si>
-    <t xml:space="preserve">この画面になったら「続ける」をクリックしてください。
- これで接続の設定が完了しました。 接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check-4&lt;/span&gt;
-  </t>
-  </si>
-  <si>
     <t>mac-3-4.png</t>
   </si>
   <si>
@@ -520,13 +510,6 @@
     <t>win10-6-06.svg</t>
   </si>
   <si>
-    <t xml:space="preserve">メールの画面が開きます。
-大学からの電子メールでの連絡は、広大メールで来ます。
-常にメールチェックするようにしてください。&lt;span class="check"&gt;check-10&lt;/span&gt;
-スマホのOutlookアプリでも、複雑な設定は必要なくメールの送受信が可能です。ここは必携PC設定の手順を示していますので、Web版をお知らせしましたが、スマホ版の方が使いやすく、新規メールが届いた時の通知もありますので、おすすめです。
-&lt;img alt="*outlook icon*" src="image/win10-outlook-app.png" width="64" /&gt;  </t>
-  </si>
-  <si>
     <t>win10-6-07.svg</t>
   </si>
   <si>
@@ -556,12 +539,6 @@
   </si>
   <si>
     <t>win10-6-10.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check-11&lt;/span&gt;
-履修登録をしたり、成績を確認することができます。
-また「掲示」では、授業や学部からの連絡が表示されます。
-  </t>
   </si>
   <si>
     <t>win10-6-11.svg</t>
@@ -640,11 +617,6 @@
   </si>
   <si>
     <t>mac-5-23.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">「大学教育入門」の第1週では、&lt;em&gt;第1章と第6章&lt;/em&gt;
-を扱いますので、同じようにして第6章に掲載されているファイルもダウンロードしておきましょう。&lt;span class="check"&gt;check-13&lt;/span&gt;
-  </t>
   </si>
   <si>
     <t>mac-5-24.png</t>
@@ -816,22 +788,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">  「Macを自動的に最新の状態に保つ」のところにチェックが入っていることを確認してください。入ってなければ入れてください。 &lt;span class="check"&gt;check-5&lt;span&gt; &lt;/span&gt;
-&lt;/span&gt;
- </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve"> 次にウイルス対策ソフトの設定を確認しましょう。 画面右上にある青い「e」のアイコンをクリックしましょう。 表示されるメニューから「ESET Endpoint Antivirus を開く」をクリックします。  
  </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve"> 「アップデート」のタブから状態を確認しましょう。 「更新は必要ありません」となっていたらOKです。&lt;span class="check"&gt;check-6,7&lt;/span&gt;
- 最新でない場合は「モジュールのアップロード」をクリックして、アップデートしましょう。 ウイルス定義データが常に最新でないと、新しいウイルスからパソコンを守ることができません。 常に最新にしておきましょう。  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve"> 次に、Officeのライセンス認証をします。ソフトウェアが正当なコピーであることを確認し、PCで使えるようにするための処理です。 Dockの中から、ロケットのアイコンの「Launchpad」をクリックしてください。  </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -863,11 +824,6 @@
   </si>
   <si>
     <t xml:space="preserve">  「今すぐWordを使ってみる」をクリックしてください。  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  Wordの新規作成の画面が開きました。 これで、PowerPointやExcelなどMicrosoft Officeの他のアプリケーションも使えるようになります。&lt;span class="check"&gt;check-9&lt;/span&gt;
-  </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1165,23 +1121,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Macにログインするときに使うパスワードを入力し、「ソフトウェアをインストール」としてください。 このあと特に警告が出なければ、&lt;a href="#chrome"&gt;Chromeを入れる&lt;/a&gt;に進んでかまいません。
-  </t>
-    <rPh sb="53" eb="54">
-      <t>トク</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>ケイコク</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="97" eb="98">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>「学生の個人所有PCへのインストールはここから」をクリックします。</t>
     <rPh sb="1" eb="3">
       <t>ガクセイ</t>
@@ -1262,22 +1201,6 @@
     </rPh>
     <rPh sb="65" eb="67">
       <t>デンゲン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">「検査プロファイル」として「詳細検査」を、「検査対象」として「Macintosh HD」を選んでください。Macintosh HDは、Macに内蔵されている副記憶装置(HDDもしくはSDD）を指します。「検査」をクリックすると、フルスキャンが始まります。&lt;span class="check"&gt;check-8&lt;span&gt;&lt;/span&gt;
-&lt;/span&gt;
-フルスキャンの実行には数時間かかりますので、時間の余裕のあるときにできるだけ早く実行し、点検届けを完成させてください。
-  </t>
-    <rPh sb="188" eb="191">
-      <t>スウジカン</t>
-    </rPh>
-    <rPh sb="199" eb="201">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="202" eb="204">
-      <t>ヨユウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1877,6 +1800,88 @@
 「大学教育入門」では、授業に参加する前に各自必携PCに教材をダウンロードしておくことが求められています。先ほど開いたメールにその旨の指示が来ていたと思います。
 ここでは、第1週に実施される講義の資料をダウンロードする手順を紹介しておきます。
 まず、コース一覧から「2020大学教育入門...」をクリックしてコースを開きましょう。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">アクティビティモニタのウィンドウで、まず「エネルギー」タブをクリックしてください。
+ この画面の下の方に、現在のバッテリー情報がかかれています。あと4時間40分使えるとあります。充電状況が100%のときにこの「残り時間」を調べれば、それがあなたのMacのバッテリー駆動時間ということになります。
+ この数字は推測値であり、プログラムの動作状況によって大きく上下することに注意してください。   </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">この画面になったら「続ける」をクリックしてください。
+ これで接続の設定が完了しました。 接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check-3&lt;/span&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wordの新規作成の画面が開きました。 これで、PowerPointやExcelなどMicrosoft Officeの他のアプリケーションも使えるようになります。&lt;span class="check"&gt;check-8&lt;/span&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Macにログインするときに使うパスワードを入力し、「ソフトウェアをインストール」としてください。 このあと特に警告が出なければ、&lt;a href="#chrome"&gt;Chromeを入れる&lt;/a&gt;に進んでかまいません。&lt;span class="check"&gt;check-5&lt;/span&gt;
+  </t>
+    <rPh sb="53" eb="54">
+      <t>トク</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ケイコク</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="97" eb="98">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  「Macを自動的に最新の状態に保つ」のところにチェックが入っていることを確認してください。入ってなければ入れてください。 &lt;span class="check"&gt;check-4&lt;span&gt; &lt;/span&gt;
+&lt;/span&gt;
+ </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「検査プロファイル」として「詳細検査」を、「検査対象」として「Macintosh HD」を選んでください。Macintosh HDは、Macに内蔵されている副記憶装置(HDDもしくはSDD）を指します。「検査」をクリックすると、フルスキャンが始まります。&lt;span class="check"&gt;check-7&lt;span&gt;&lt;/span&gt;
+&lt;/span&gt;
+フルスキャンの実行には数時間かかりますので、時間の余裕のあるときにできるだけ早く実行し、点検届を完成させてください。
+  </t>
+    <rPh sb="188" eb="191">
+      <t>スウジカン</t>
+    </rPh>
+    <rPh sb="199" eb="201">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="202" eb="204">
+      <t>ヨユウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 「アップデート」のタブから状態を確認しましょう。 「更新は必要ありません」となっていたらOKです。&lt;span class="check"&gt;check-6&lt;/span&gt;
+ 最新でない場合は「モジュールのアップロード」をクリックして、アップデートしましょう。 ウイルス定義データが常に最新でないと、新しいウイルスからパソコンを守ることができません。 常に最新にしておきましょう。  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">メールの画面が開きます。
+大学からの電子メールでの連絡は、広大メールで来ます。
+常にメールチェックするようにしてください。&lt;span class="check"&gt;check-9&lt;/span&gt;
+スマホのOutlookアプリでも、複雑な設定は必要なくメールの送受信が可能です。ここは必携PC設定の手順を示していますので、Web版をお知らせしましたが、スマホ版の方が使いやすく、新規メールが届いた時の通知もありますので、おすすめです。
+&lt;img alt="*outlook icon*" src="image/win10-outlook-app.png" width="64" /&gt;  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check-10&lt;/span&gt;
+履修登録をしたり、成績を確認することができます。
+また「掲示」では、授業や学部からの連絡が表示されます。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「大学教育入門」の第1週では、&lt;em&gt;第1章と第6章&lt;/em&gt;
+を扱いますので、同じようにして第6章に掲載されているファイルもダウンロードしておきましょう。&lt;span class="check"&gt;check-11&lt;/span&gt;
   </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2286,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2302,7 +2307,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2310,7 +2315,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -2361,7 +2366,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2369,7 +2374,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2385,7 +2390,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2393,7 +2398,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2404,7 +2409,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2412,13 +2417,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2426,13 +2431,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -2440,13 +2445,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2454,18 +2459,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2473,13 +2478,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2487,13 +2492,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2501,13 +2506,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2515,13 +2520,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2529,13 +2534,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2543,13 +2548,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2557,18 +2562,18 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2576,13 +2581,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2590,13 +2595,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2604,13 +2609,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2618,13 +2623,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2632,13 +2637,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2646,13 +2651,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2660,13 +2665,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2674,13 +2679,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2688,13 +2693,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2702,13 +2707,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2716,13 +2721,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2730,13 +2735,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2744,13 +2749,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2758,13 +2763,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2772,13 +2777,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2786,13 +2791,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2800,13 +2805,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2814,18 +2819,18 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="130" x14ac:dyDescent="0.2">
@@ -2833,13 +2838,13 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2847,7 +2852,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -2895,7 +2900,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2919,7 +2924,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3128,8 +3133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3169,7 +3174,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3205,13 +3210,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3256,18 +3261,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>293</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3281,8 +3286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3298,7 +3303,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3306,7 +3311,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3322,12 +3327,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3335,13 +3340,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3349,13 +3354,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3363,13 +3368,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3377,13 +3382,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>55</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -3391,13 +3396,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3405,13 +3410,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>294</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3425,8 +3430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="B18" zoomScale="113" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="B28" zoomScale="113" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3442,7 +3447,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3450,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3466,7 +3471,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3474,7 +3479,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3485,12 +3490,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3498,13 +3503,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3512,13 +3517,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3526,37 +3531,37 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="D12" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D13" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D14" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3564,18 +3569,18 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3583,13 +3588,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3597,13 +3602,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3611,13 +3616,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3625,13 +3630,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3639,13 +3644,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3653,18 +3658,18 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3672,13 +3677,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3686,13 +3691,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3700,13 +3705,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3714,13 +3719,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3728,13 +3733,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3742,13 +3747,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3756,13 +3761,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3770,13 +3775,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3784,13 +3789,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>216</v>
+        <v>295</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3798,13 +3803,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3812,13 +3817,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -3826,13 +3831,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3845,8 +3850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACFDDE6-1E06-4807-90D9-56730BF2F634}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" zoomScale="138" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="B24" zoomScale="138" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3862,7 +3867,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3870,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3886,7 +3891,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3894,7 +3899,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3905,23 +3910,23 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D8" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D9" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3929,26 +3934,26 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="D12" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3956,34 +3961,34 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="D14" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="D15" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3991,13 +3996,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4005,13 +4010,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4019,13 +4024,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4033,13 +4038,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4047,13 +4052,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4061,13 +4066,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4075,13 +4080,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4089,13 +4094,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4103,13 +4108,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4117,13 +4122,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4131,13 +4136,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>243</v>
+        <v>296</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4145,13 +4150,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4159,13 +4164,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4173,13 +4178,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4187,13 +4192,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4201,13 +4206,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4215,13 +4220,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4229,13 +4234,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -4249,8 +4254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4266,7 +4271,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4274,7 +4279,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4290,7 +4295,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4298,7 +4303,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4309,7 +4314,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4317,13 +4322,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4331,13 +4336,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4345,18 +4350,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>205</v>
+        <v>297</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4364,13 +4369,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4378,13 +4383,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>207</v>
+        <v>299</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4392,13 +4397,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4406,13 +4411,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>251</v>
+        <v>298</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -4426,8 +4431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4443,7 +4448,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4451,7 +4456,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4467,7 +4472,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -4475,7 +4480,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4486,7 +4491,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4508,13 +4513,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4522,18 +4527,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4555,13 +4560,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4569,21 +4574,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4591,13 +4596,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4605,13 +4610,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" t="s">
         <v>135</v>
-      </c>
-      <c r="C17" t="s">
-        <v>136</v>
-      </c>
-      <c r="D17" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4619,13 +4624,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4633,13 +4638,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>140</v>
+        <v>300</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4647,13 +4652,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4661,18 +4666,18 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -4694,13 +4699,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4708,13 +4713,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>149</v>
+        <v>301</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4722,18 +4727,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -4755,13 +4760,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4769,13 +4774,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4783,13 +4788,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4797,13 +4802,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -4811,13 +4816,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4825,13 +4830,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4839,13 +4844,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4853,13 +4858,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4867,13 +4872,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4881,18 +4886,18 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>170</v>
+        <v>302</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4900,7 +4905,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -4914,13 +4919,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4928,13 +4933,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C42" t="s">
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4942,13 +4947,13 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -4956,13 +4961,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -4990,10 +4995,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5001,7 +5006,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5017,7 +5022,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5025,7 +5030,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5036,12 +5041,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5049,7 +5054,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -5060,7 +5065,7 @@
     </row>
     <row r="10" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win10e/mac/win8.1 Ch5 to change pdf download check
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508AC9D9-0AB9-43FC-95D4-48D76A328E96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1EC766-84C1-4BE1-B6C1-5A8A01423EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29295" yWindow="2070" windowWidth="17925" windowHeight="12450" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35055" yWindow="2535" windowWidth="13425" windowHeight="10575" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="300">
   <si>
     <t>header1</t>
   </si>
@@ -588,38 +588,6 @@
   </si>
   <si>
     <t>win10-6-17.svg</t>
-  </si>
-  <si>
-    <t>win10-6-18.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">左メニューの「テキスト・スライド資料」をクリックすると右側にフォルダが表示されます。各週の資料がまとめられていますね。
-「第1章　大学で何を学ぶか（各学部・プログラム）」をクリックして開きましょう。
-  </t>
-  </si>
-  <si>
-    <t>mac-5-21.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">フォルダの中には三つのファイルがあります。
-ファイルのリンクをクリックすると、この場で内容を確認できます。
-授業の準備として事前にダウンロードしたい場合は、リンクを右クリックします。
-右クリックして表示されるメニューから「リンク先のファイルをダウンロード」としてください。
-  </t>
-  </si>
-  <si>
-    <t>mac-5-22.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">同様にして三つのファイルをダウンロードします。ダウンロードしたファイルはドックの右端、ゴミ箱の左隣からアクセスできます。そこをクリックすると、これまでダウンロードしたファイルが図のように表示されます。
-Safariを開いている時であれば、ウィンドウ上方の下向き矢印アイコンからもアクセスできます。
-  </t>
-  </si>
-  <si>
-    <t>mac-5-23.png</t>
-  </si>
-  <si>
-    <t>mac-5-24.png</t>
   </si>
   <si>
     <t>&lt;h2&gt;&lt;a name="omake"&gt;&lt;/a&gt;おまけ&lt;/h2&gt;</t>
@@ -1780,30 +1748,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">2回目からはログインしたら、この画面が出ます。
-真ん中の「コース一覧」に、あなたがアクセスできるコースが表示されています。
-ここに並んでいるコースは、あなたが受講する授業に関連したものと、そうでないものがあります。今並んでいるものを簡単に説明すると：
-&lt;dl&gt;&lt;dt&gt;大学教育入門&lt;/dt&gt;
-&lt;dd&gt;「大学教育入門」は、大学で学ぶにあたり必要な事柄や、広島大学特有の事情について学習する授業です。全学部生必修です。このコースでは、授業の各週で使う資料をダウンロードしたり、確認テストを受験したりします。&lt;/dd&gt;
-&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
-&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届け」を提出する必要があります。このコースでは、点検届けが提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
-&lt;dt&gt;Information Security and Compliance (情報セキュリティ・コンプライアンス)&lt;/dt&gt;
-&lt;dd&gt;「情報セキュリティ・コンプライアンス講習」は、広島大学でパソコンやネットワークを安全に使うための講座です。学生だけでなく、教職員を含めた全構成員必修の内容です。講習は、教室での講義とオンライン学習（このコース）からなっています。6月末までにこのコースの中にある確認テストに合格し、「&lt;em&gt;アカウント利用確認&lt;/em&gt;
-」の手続きをおこなわないと、アカウントがロックされ、メール等が使えなくなります。&lt;/dd&gt;
- &lt;/dl&gt;
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Bb9で配布されている教材を開けることを確認するため、「大学教育入門」のコースをみてみましょう。
-転入生の方は、「大学教育入門」がありませんので、「Information Security and Compliance」のコースを開いて、スライドなどがみられることを確認してください。
-「大学教育入門」では、授業に参加する前に各自必携PCに教材をダウンロードしておくことが求められています。先ほど開いたメールにその旨の指示が来ていたと思います。
-ここでは、第1週に実施される講義の資料をダウンロードする手順を紹介しておきます。
-まず、コース一覧から「2020大学教育入門...」をクリックしてコースを開きましょう。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">アクティビティモニタのウィンドウで、まず「エネルギー」タブをクリックしてください。
  この画面の下の方に、現在のバッテリー情報がかかれています。あと4時間40分使えるとあります。充電状況が100%のときにこの「残り時間」を調べれば、それがあなたのMacのバッテリー駆動時間ということになります。
  この数字は推測値であり、プログラムの動作状況によって大きく上下することに注意してください。   </t>
@@ -1880,9 +1824,233 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">「大学教育入門」の第1週では、&lt;em&gt;第1章と第6章&lt;/em&gt;
-を扱いますので、同じようにして第6章に掲載されているファイルもダウンロードしておきましょう。&lt;span class="check"&gt;check-11&lt;/span&gt;
-  </t>
+    <t>2回目からはログインしたら、この画面が出ます。
+真ん中の「コース一覧」に、あなたがアクセスできるコースが表示されています。
+これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。新入生共通で表示されるものを簡単に説明すると：
+&lt;dl&gt;
+&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
+&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届」を提出する必要があります。このコースでは、点検届が提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
+&lt;dt&gt;大学教育入門&lt;/dt&gt;
+&lt;dd&gt;「大学教育入門」は、大学で学ぶにあたり必要な事柄や、広島大学特有の事情について学習する授業です。全学部生必修です。このコースでは、授業の各週で使う資料をダウンロードしたり、確認テストを受験したりします。&lt;/dd&gt; &lt;/dl&gt;
+  &lt;p class="spl"&gt;※今年の「大学教育入門」は、新型コロナウィルス対策のために受講方法が例年と異なります。「もみじ」などでの案内によく注意してください。&lt;/p&gt;</t>
+    <rPh sb="71" eb="73">
+      <t>リシュウ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>カモク</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>シエン</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="93" eb="95">
+      <t>ジシュウ</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="109" eb="112">
+      <t>シンニュウセイ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="262" eb="264">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="265" eb="267">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="268" eb="269">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="280" eb="281">
+      <t>ハヤ</t>
+    </rPh>
+    <rPh sb="289" eb="290">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="471" eb="473">
+      <t>コトシ</t>
+    </rPh>
+    <rPh sb="475" eb="477">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="477" eb="479">
+      <t>キョウイク</t>
+    </rPh>
+    <rPh sb="479" eb="481">
+      <t>ニュウモン</t>
+    </rPh>
+    <rPh sb="484" eb="486">
+      <t>シンガタ</t>
+    </rPh>
+    <rPh sb="493" eb="495">
+      <t>タイサク</t>
+    </rPh>
+    <rPh sb="499" eb="501">
+      <t>ジュコウ</t>
+    </rPh>
+    <rPh sb="501" eb="503">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="504" eb="506">
+      <t>レイネン</t>
+    </rPh>
+    <rPh sb="507" eb="508">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="522" eb="524">
+      <t>アンナイ</t>
+    </rPh>
+    <rPh sb="527" eb="529">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Bb9で配布されている教材をダウンロードできることを確認するため、「ノートパソコン点検届」のコースをみてみましょう。
+まず、コース一覧から「ノートパソコン点検届2020」をクリックしてコースを開きましょう。
+  </t>
+    <rPh sb="41" eb="43">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="79" eb="80">
+      <t>トドケ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">左メニューの「教材」をクリックすると右側にフォルダが表示されます。いちばん上は、点検届を提出するためのリンクです。
+２番目にある「点検届ワークシート/Checklist worksheet」をクリックして開きましょう。
+  </t>
+    <rPh sb="7" eb="9">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>テイシュツ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>バンメ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>トドケ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">このようにPDFファイルの内容が表示されます。使っているソフト（「環境」といったりしますね）によっては、画面に直接表示されない場合もあります。そのときは、「ここをクリックして〇〇を開いてください」をクリックします。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-31.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">掲載されているファイルを保存（ダウンロード）する一番簡単な方法は、この画面で表示内容を右クリックして保存することです。
+左クリックして表示されるメニューから「名前を付けて保存」をクリックします。
+  </t>
+    <rPh sb="38" eb="40">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="82" eb="83">
+      <t>ツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-32.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このテキストの第１章からここまで順に進んでいれば、点検届チェックリストがすべてチェックできているはずです。&lt;strong&gt;Bb9の「ノートパソコン点検届」コースを開いて、点検届を提出しましょう！&lt;/strong&gt;</t>
+    <rPh sb="7" eb="8">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ジュン</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="81" eb="82">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="87" eb="88">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="89" eb="91">
+      <t>テイシュツ</t>
+    </rPh>
+    <rPh sb="111" eb="112">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="155" eb="156">
+      <t>スス</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2291,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2307,7 +2475,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2315,7 +2483,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -2366,7 +2534,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2374,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2390,7 +2558,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2398,7 +2566,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2409,7 +2577,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2417,13 +2585,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2431,13 +2599,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -2445,13 +2613,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2459,18 +2627,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2478,13 +2646,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2492,7 +2660,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2520,7 +2688,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -2534,7 +2702,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2562,7 +2730,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2581,7 +2749,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -2637,7 +2805,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -2651,7 +2819,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -2721,7 +2889,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -2735,7 +2903,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -2805,7 +2973,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -2838,13 +3006,13 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2852,7 +3020,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -2900,7 +3068,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2924,7 +3092,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3174,7 +3342,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3210,13 +3378,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3266,7 +3434,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -3327,12 +3495,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3340,7 +3508,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3354,7 +3522,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -3410,7 +3578,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -3447,7 +3615,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3455,7 +3623,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3471,7 +3639,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3479,7 +3647,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3490,12 +3658,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3503,13 +3671,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3517,13 +3685,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3531,37 +3699,37 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D12" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D13" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D14" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3569,18 +3737,18 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3588,7 +3756,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -3616,7 +3784,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -3630,7 +3798,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -3658,7 +3826,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -3669,7 +3837,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3677,7 +3845,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -3691,7 +3859,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -3705,7 +3873,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -3719,7 +3887,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -3733,7 +3901,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -3747,7 +3915,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -3761,7 +3929,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -3775,7 +3943,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -3789,7 +3957,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -3803,7 +3971,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -3817,13 +3985,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -3831,7 +3999,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -3867,7 +4035,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3875,7 +4043,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3891,7 +4059,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3899,7 +4067,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3915,18 +4083,18 @@
     </row>
     <row r="8" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D8" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D9" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3934,13 +4102,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3950,10 +4118,10 @@
     </row>
     <row r="12" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D12" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3961,34 +4129,34 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D14" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D15" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3996,7 +4164,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -4024,7 +4192,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -4052,7 +4220,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -4066,7 +4234,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -4136,7 +4304,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -4150,7 +4318,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -4220,7 +4388,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -4295,7 +4463,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4303,7 +4471,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4322,7 +4490,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -4336,7 +4504,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -4350,7 +4518,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -4361,7 +4529,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4369,7 +4537,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -4383,7 +4551,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -4397,7 +4565,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -4411,7 +4579,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -4431,8 +4599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4472,7 +4640,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -4480,7 +4648,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4585,10 +4753,10 @@
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4596,13 +4764,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4638,7 +4806,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -4713,7 +4881,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -4811,12 +4979,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="234" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="182" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -4825,18 +4993,15 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4844,27 +5009,24 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>160</v>
+        <v>294</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
-      <c r="D35" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>162</v>
+        <v>295</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>163</v>
+        <v>296</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4872,32 +5034,26 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>164</v>
+        <v>297</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" t="s">
-        <v>166</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4905,7 +5061,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -4919,13 +5075,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4933,13 +5089,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C42" t="s">
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4947,13 +5103,13 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -4961,13 +5117,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -4995,10 +5151,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5006,7 +5162,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5022,7 +5178,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5030,7 +5186,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5041,12 +5197,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5054,7 +5210,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -5065,7 +5221,7 @@
     </row>
     <row r="10" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
macs ch5 fix Command-S
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1EC766-84C1-4BE1-B6C1-5A8A01423EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F3D1E17-4846-44FC-A6A9-4C35D653B13F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35055" yWindow="2535" windowWidth="13425" windowHeight="10575" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31875" yWindow="2880" windowWidth="13425" windowHeight="10575" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,12 @@
     <sheet name="ch8" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="299">
   <si>
     <t>header1</t>
   </si>
@@ -1980,31 +1981,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">掲載されているファイルを保存（ダウンロード）する一番簡単な方法は、この画面で表示内容を右クリックして保存することです。
-左クリックして表示されるメニューから「名前を付けて保存」をクリックします。
-  </t>
-    <rPh sb="38" eb="40">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="50" eb="52">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>ナマエ</t>
-    </rPh>
-    <rPh sb="82" eb="83">
-      <t>ツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-6-32.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>このテキストの第１章からここまで順に進んでいれば、点検届チェックリストがすべてチェックできているはずです。&lt;strong&gt;Bb9の「ノートパソコン点検届」コースを開いて、点検届を提出しましょう！&lt;/strong&gt;</t>
     <rPh sb="7" eb="8">
       <t>ダイ</t>
@@ -2040,16 +2016,33 @@
       <t>トドケ</t>
     </rPh>
     <rPh sb="89" eb="91">
-      <t>テイシュツ</t>
-    </rPh>
-    <rPh sb="111" eb="112">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="115" eb="117">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="155" eb="156">
-      <t>スス</t>
+      <t>テイシュツツカバアイスス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">表示されているファイルを保存（ダウンロード）する一番簡単な方法は、この画面でCommand-Sを入力して保存することです。
+書き出し名を指定して保存します。  </t>
+    <rPh sb="48" eb="50">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ホゾン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4423,7 +4416,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4599,8 +4592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -5029,18 +5022,15 @@
         <v>296</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -5048,7 +5038,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add pics Checklist submit and ESET download
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F3D1E17-4846-44FC-A6A9-4C35D653B13F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A8636D-09EA-4A16-93DE-7B6D9AE8C7E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31875" yWindow="2880" windowWidth="13425" windowHeight="10575" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,11 @@
     <sheet name="ch8" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="301">
   <si>
     <t>header1</t>
   </si>
@@ -1972,11 +1971,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">このようにPDFファイルの内容が表示されます。使っているソフト（「環境」といったりしますね）によっては、画面に直接表示されない場合もあります。そのときは、「ここをクリックして〇〇を開いてください」をクリックします。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win10-6-31.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2021,29 +2015,22 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">表示されているファイルを保存（ダウンロード）する一番簡単な方法は、この画面でCommand-Sを入力して保存することです。
-書き出し名を指定して保存します。  </t>
-    <rPh sb="48" eb="50">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="64" eb="65">
-      <t>ダ</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ホゾン</t>
-    </rPh>
+    <t>mac-4-31.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-34.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">このようにPDFファイルの内容が表示されます。使っているソフト（「環境」といったりしますね）によっては、画面に直接表示されない場合もあります。そのときは、「ここをクリックして〇〇を開いてください」をクリックします。
+PDFファイルを保存（ダウンロード）する一番簡単な方法は、PDFが表示されているこの画面でCommand-Sを入力して保存することです。
+書き出し名を指定して保存します。  &lt;span class="check"&gt;check-11&lt;/span&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-35.svg</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4011,8 +3998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACFDDE6-1E06-4807-90D9-56730BF2F634}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="B24" zoomScale="138" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="C11" zoomScale="134" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4151,6 +4138,9 @@
       <c r="B16" s="1" t="s">
         <v>225</v>
       </c>
+      <c r="D16" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -4415,8 +4405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4590,10 +4580,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -5007,112 +4997,107 @@
       <c r="C35" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
         <v>295</v>
       </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
+    </row>
+    <row r="37" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
+      <c r="D37" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
       <c r="B39" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="117" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C42" t="s">
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add caution to postpone HINET network connection check
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A8636D-09EA-4A16-93DE-7B6D9AE8C7E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5913F1E8-BE9F-4DC6-952F-ED058310B189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31875" yWindow="2880" windowWidth="13425" windowHeight="10575" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33675" yWindow="1065" windowWidth="23070" windowHeight="10575" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="302">
   <si>
     <t>header1</t>
   </si>
@@ -2031,6 +2031,93 @@
   </si>
   <si>
     <t>win10-6-35.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;strong&gt;新型コロナウィルス対策のため、対面型授業開始（５月連休明けを予定）までは、大学キャンパスへの来校は必要最小限の用事があるときのみとなります。
+したがって、この章の作業は後回しにしていただいてかまいません。来校して時間の余裕のあるときに行ってください。&lt;/strong&gt;
+&lt;p class="spl"&gt;※学生証に書かれている学生番号と、学生証と一緒にもらえる「広大パスワード」が必要です。&lt;/p&gt;</t>
+    <rPh sb="8" eb="10">
+      <t>シンガタ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>タイサク</t>
+    </rPh>
+    <rPh sb="23" eb="26">
+      <t>タイメンガタ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ガツ</t>
+    </rPh>
+    <rPh sb="33" eb="36">
+      <t>レンキュウア</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ヨテイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>ライコウ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="59" eb="62">
+      <t>サイショウゲン</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>ヨウジ</t>
+    </rPh>
+    <rPh sb="92" eb="93">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>マワ</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>ライコウ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>ヨユウ</t>
+    </rPh>
+    <rPh sb="125" eb="126">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="159" eb="162">
+      <t>ガクセイショウ</t>
+    </rPh>
+    <rPh sb="163" eb="164">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="169" eb="171">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="171" eb="173">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="175" eb="178">
+      <t>ガクセイショウ</t>
+    </rPh>
+    <rPh sb="179" eb="181">
+      <t>イッショ</t>
+    </rPh>
+    <rPh sb="187" eb="189">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="196" eb="198">
+      <t>ヒツヨウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3432,10 +3519,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3484,86 +3571,91 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
       <c r="B7" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="117" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4582,8 +4674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix about HINET network
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5913F1E8-BE9F-4DC6-952F-ED058310B189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9654EDC6-D7C9-4700-A7DB-357DFAB67701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33675" yWindow="1065" windowWidth="23070" windowHeight="10575" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -2034,8 +2034,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;strong&gt;新型コロナウィルス対策のため、対面型授業開始（５月連休明けを予定）までは、大学キャンパスへの来校は必要最小限の用事があるときのみとなります。
-したがって、この章の作業は後回しにしていただいてかまいません。来校して時間の余裕のあるときに行ってください。&lt;/strong&gt;
+    <t>&lt;strong&gt;新型コロナウィルス対策のため、この章の作業は後回しにしていただいてかまいません。来校して時間の余裕のあるときに行ってください。&lt;/strong&gt;
 &lt;p class="spl"&gt;※学生証に書かれている学生番号と、学生証と一緒にもらえる「広大パスワード」が必要です。&lt;/p&gt;</t>
     <rPh sb="8" eb="10">
       <t>シンガタ</t>
@@ -2043,79 +2042,46 @@
     <rPh sb="17" eb="19">
       <t>タイサク</t>
     </rPh>
-    <rPh sb="23" eb="26">
-      <t>タイメンガタ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>ガツ</t>
-    </rPh>
-    <rPh sb="33" eb="36">
-      <t>レンキュウア</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>ヨテイ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="54" eb="56">
+    <rPh sb="30" eb="31">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>マワ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
       <t>ライコウ</t>
     </rPh>
-    <rPh sb="57" eb="59">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="59" eb="62">
-      <t>サイショウゲン</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>ヨウジ</t>
-    </rPh>
-    <rPh sb="92" eb="93">
-      <t>アト</t>
-    </rPh>
-    <rPh sb="93" eb="94">
-      <t>マワ</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>ライコウ</t>
-    </rPh>
-    <rPh sb="114" eb="116">
+    <rPh sb="52" eb="54">
       <t>ジカン</t>
     </rPh>
+    <rPh sb="55" eb="57">
+      <t>ヨユウ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="97" eb="100">
+      <t>ガクセイショウ</t>
+    </rPh>
+    <rPh sb="101" eb="102">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="109" eb="111">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="113" eb="116">
+      <t>ガクセイショウ</t>
+    </rPh>
     <rPh sb="117" eb="119">
-      <t>ヨユウ</t>
-    </rPh>
-    <rPh sb="125" eb="126">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="159" eb="162">
-      <t>ガクセイショウ</t>
-    </rPh>
-    <rPh sb="163" eb="164">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="169" eb="171">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="171" eb="173">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="175" eb="178">
-      <t>ガクセイショウ</t>
-    </rPh>
-    <rPh sb="179" eb="181">
       <t>イッショ</t>
     </rPh>
-    <rPh sb="187" eb="189">
+    <rPh sb="125" eb="127">
       <t>ヒロダイ</t>
     </rPh>
-    <rPh sb="196" eb="198">
+    <rPh sb="134" eb="136">
       <t>ヒツヨウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -3522,7 +3488,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3570,7 +3536,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>301</v>
       </c>

</xml_diff>

<commit_message>
update screenshot of the link to portal.office.com
</commit_message>
<xml_diff>
--- a/macs.xlsx
+++ b/macs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2021_03\初期講習会\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95104B07-D234-44F2-8153-6FBE10AF6569}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1525B43-F4ED-47A2-9B78-A69327150C13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6396" tabRatio="772" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6396" tabRatio="772" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,11 @@
     <sheet name="ch9" sheetId="16" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="322">
   <si>
     <t>header1</t>
   </si>
@@ -233,13 +232,6 @@
   </si>
   <si>
     <t>win10-6-27.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">最初の一回だけ、使用言語とタイムゾーンを選ぶ画面が出ます。通常は「日本語」と「UTC+9」を選んでおけば良いでしょう。 
-  </t>
-  </si>
-  <si>
-    <t>win10-6-06.svg</t>
   </si>
   <si>
     <t>win10-6-07.svg</t>
@@ -4627,7 +4619,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4643,7 +4635,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -4651,7 +4643,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -4699,10 +4691,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4710,7 +4702,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4726,7 +4718,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4734,7 +4726,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4745,12 +4737,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="211.2" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4758,7 +4750,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -4769,7 +4761,7 @@
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -4800,7 +4792,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4808,7 +4800,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4824,7 +4816,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -4832,7 +4824,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4846,7 +4838,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4856,13 +4848,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -4870,24 +4862,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4895,13 +4887,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4909,40 +4901,40 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -4950,13 +4942,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -4964,24 +4956,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D20" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -4989,13 +4981,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5003,35 +4995,35 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5039,13 +5031,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5053,18 +5045,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -5095,7 +5087,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5119,7 +5111,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5147,7 +5139,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5155,13 +5147,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5169,24 +5161,24 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5194,13 +5186,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5208,13 +5200,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5228,18 +5220,18 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5247,13 +5239,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5267,7 +5259,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5281,7 +5273,7 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -5289,134 +5281,134 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -5424,13 +5416,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -5485,7 +5477,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -5493,7 +5485,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5507,13 +5499,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -5521,13 +5513,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -5535,13 +5527,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -5549,13 +5541,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5563,24 +5555,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5588,24 +5580,24 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -5660,17 +5652,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5678,7 +5670,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -5692,7 +5684,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -5748,7 +5740,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -5785,7 +5777,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5793,7 +5785,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5809,7 +5801,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5817,7 +5809,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5828,18 +5820,18 @@
     </row>
     <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -5847,13 +5839,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -5884,7 +5876,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5892,7 +5884,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5908,20 +5900,20 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -5929,37 +5921,37 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5967,18 +5959,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6094,7 +6086,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6102,7 +6094,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6118,7 +6110,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -6126,7 +6118,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6137,12 +6129,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -6150,13 +6142,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6164,18 +6156,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" t="s">
         <v>261</v>
-      </c>
-      <c r="D10" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6183,53 +6175,53 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D17" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6237,13 +6229,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6257,7 +6249,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6265,13 +6257,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6279,13 +6271,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6293,13 +6285,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6307,18 +6299,18 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6326,7 +6318,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -6340,7 +6332,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -6354,7 +6346,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -6368,7 +6360,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -6382,7 +6374,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -6396,7 +6388,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -6410,7 +6402,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -6424,7 +6416,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -6438,7 +6430,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -6452,7 +6444,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -6466,13 +6458,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -6480,7 +6472,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -6499,7 +6491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -6516,7 +6508,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6524,7 +6516,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6540,7 +6532,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -6548,7 +6540,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6567,7 +6559,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6581,7 +6573,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -6595,34 +6587,34 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6630,7 +6622,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -6644,7 +6636,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -6655,10 +6647,10 @@
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6666,7 +6658,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -6680,7 +6672,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -6698,10 +6690,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B34" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6741,7 +6733,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="237.6" x14ac:dyDescent="0.2">
@@ -6749,7 +6741,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6843,21 +6835,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6865,13 +6857,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6888,26 +6880,26 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -6916,7 +6908,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -6930,59 +6922,59 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>68</v>
       </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -6991,40 +6983,40 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -7038,7 +7030,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -7049,135 +7041,135 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>78</v>
       </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
         <v>79</v>
       </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
+    <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D37" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C40" t="s">
         <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -7191,7 +7183,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -7203,20 +7195,6 @@
       </c>
       <c r="D42" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>